<commit_message>
Making the quality apprisal
</commit_message>
<xml_diff>
--- a/4_Classification/Classified_Studies.xlsx
+++ b/4_Classification/Classified_Studies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antoniotrovato/Documents/GitHub/RegressionTestingOptimizationSLR/4_Classification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCE7017E-CC56-7C4D-BE4F-EE922131D843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DE2C2C2-73EC-5E49-945C-58F8A05BF7E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9940" yWindow="660" windowWidth="28800" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3240,8 +3240,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AN110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="A110" sqref="A110:XFD110"/>
+    <sheetView tabSelected="1" topLeftCell="AF1" workbookViewId="0">
+      <selection activeCell="AN20" sqref="AN20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4156,7 +4156,7 @@
         <v>852</v>
       </c>
       <c r="AN20" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
     </row>
     <row r="21" spans="1:40" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update study counts and quality appraisal info
Updated counts of primary studies and surveys/reviews in 4_Classification/Info.rtf. Revised quality appraisal info in 6_Quality Appraisal/info.rtf to include the number of selected papers. Added 7_Data_Extraction/info.rtf to document removed extended work. Updated several Excel and Word documents with new data.
</commit_message>
<xml_diff>
--- a/4_Classification/Classified_Studies.xlsx
+++ b/4_Classification/Classified_Studies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antoniotrovato/Documents/GitHub/RegressionTestingOptimizationSLR/4_Classification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DE2C2C2-73EC-5E49-945C-58F8A05BF7E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C091BB7E-5185-EB40-8316-BE78D6ACE8D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9940" yWindow="660" windowWidth="28800" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3240,8 +3240,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AN110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AF1" workbookViewId="0">
-      <selection activeCell="AN20" sqref="AN20"/>
+    <sheetView tabSelected="1" topLeftCell="AG72" workbookViewId="0">
+      <selection activeCell="AN97" sqref="AN97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4733,7 +4733,7 @@
         <v>866</v>
       </c>
       <c r="AN34" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
     </row>
     <row r="35" spans="1:40" x14ac:dyDescent="0.2">
@@ -7388,7 +7388,7 @@
         <v>929</v>
       </c>
       <c r="AN97" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
     </row>
     <row r="98" spans="1:40" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Quality appraisal and data extraction finished.
</commit_message>
<xml_diff>
--- a/4_Classification/Classified_Studies.xlsx
+++ b/4_Classification/Classified_Studies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antoniotrovato/Documents/GitHub/RegressionTestingOptimizationSLR/4_Classification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C091BB7E-5185-EB40-8316-BE78D6ACE8D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DE2C2C2-73EC-5E49-945C-58F8A05BF7E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9940" yWindow="660" windowWidth="28800" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3240,8 +3240,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AN110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AG72" workbookViewId="0">
-      <selection activeCell="AN97" sqref="AN97"/>
+    <sheetView tabSelected="1" topLeftCell="AF1" workbookViewId="0">
+      <selection activeCell="AN20" sqref="AN20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4733,7 +4733,7 @@
         <v>866</v>
       </c>
       <c r="AN34" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
     </row>
     <row r="35" spans="1:40" x14ac:dyDescent="0.2">
@@ -7388,7 +7388,7 @@
         <v>929</v>
       </c>
       <c r="AN97" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
     </row>
     <row r="98" spans="1:40" x14ac:dyDescent="0.2">
@@ -8040,4 +8040,231 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100B6889C2593FACB4192549183B8B19287" ma:contentTypeVersion="11" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="8f919e2780f892880bff7efb43d3db1d">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ab92c565-5003-4ac3-93a3-a3ce8796a3c0" xmlns:ns3="aa1b21cb-23df-461b-8b8e-4aaeac2f3f50" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1ca4d89da73e1329ebe7ff2e4ed471c6" ns2:_="" ns3:_="">
+    <xsd:import namespace="ab92c565-5003-4ac3-93a3-a3ce8796a3c0"/>
+    <xsd:import namespace="aa1b21cb-23df-461b-8b8e-4aaeac2f3f50"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="ab92c565-5003-4ac3-93a3-a3ce8796a3c0" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="10" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="11" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="13" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Tag immagine" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="75195dc1-fe89-472b-8717-1a0640488213" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="15" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="16" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="17" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="18" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="aa1b21cb-23df-461b-8b8e-4aaeac2f3f50" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="TaxCatchAll" ma:index="14" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{9d5b2749-c0c4-4483-901e-60ca1fd7f0c8}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="aa1b21cb-23df-461b-8b8e-4aaeac2f3f50">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Tipo di contenuto"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Titolo"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ab92c565-5003-4ac3-93a3-a3ce8796a3c0">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="aa1b21cb-23df-461b-8b8e-4aaeac2f3f50" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA9B750E-32A4-4B1C-8C32-0B964EAA798D}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB5BF9A8-31B9-47BB-B2C0-4B65DE275DC5}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F67ACDF3-52F9-4F2F-9CDF-3164D8FC7704}"/>
 </file>
</xml_diff>